<commit_message>
base code only simulation
</commit_message>
<xml_diff>
--- a/results/agv_logs_M1.xlsx
+++ b/results/agv_logs_M1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -481,7 +481,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>J27</t>
+          <t>J1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -491,7 +491,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>71</v>
+        <v>291.3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -505,7 +505,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>J21</t>
+          <t>J7</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -515,7 +515,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>84</v>
+        <v>404.4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -529,7 +529,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>J5</t>
+          <t>J18</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
@@ -539,7 +539,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>115</v>
+        <v>417.4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -553,7 +553,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>J29</t>
+          <t>J7</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -563,7 +563,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>128</v>
+        <v>503.5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>J1</t>
+          <t>J29</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -587,7 +587,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>154</v>
+        <v>534.5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -601,7 +601,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>J26</t>
+          <t>J7</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -611,7 +611,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>169.3999999999999</v>
+        <v>616.6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -635,7 +635,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>178.4999999999999</v>
+        <v>781.8000000000001</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>J20</t>
+          <t>J13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
@@ -659,7 +659,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>201.5999999999999</v>
+        <v>979.0000000000001</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>J6</t>
+          <t>J25</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -683,7 +683,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>210.6999999999999</v>
+        <v>1147.2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -697,7 +697,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>J28</t>
+          <t>J9</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>233.7999999999999</v>
+        <v>1253.3</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>J12</t>
+          <t>J10</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
@@ -731,7 +731,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>267.8999999999999</v>
+        <v>1259.3</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -745,7 +745,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>J2</t>
+          <t>J9</t>
         </is>
       </c>
       <c r="E13" t="inlineStr"/>
@@ -755,7 +755,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>280.8999999999999</v>
+        <v>1359.4</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -779,7 +779,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>286.8999999999999</v>
+        <v>1503.6</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -793,7 +793,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>J24</t>
+          <t>J2</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
@@ -803,7 +803,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>306.6</v>
+        <v>1583.799999999999</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>J10</t>
+          <t>J2</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
@@ -827,7 +827,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>338.8</v>
+        <v>1822.099999999999</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -841,7 +841,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>J8</t>
+          <t>J3</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
@@ -851,7 +851,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>351.8</v>
+        <v>1990.299999999999</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>J9</t>
+          <t>J5</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -875,7 +875,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>383.0000000000003</v>
+        <v>2196.599999999999</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -889,7 +889,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>J5</t>
+          <t>J11</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
@@ -899,7 +899,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>426.0000000000003</v>
+        <v>2361.799999999999</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -913,7 +913,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>J20</t>
+          <t>J28</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
@@ -923,7 +923,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>494.0000000000003</v>
+        <v>2555.099999999999</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>J29</t>
+          <t>J24</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
@@ -947,7 +947,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>539.6000000000008</v>
+        <v>2561.099999999999</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -961,7 +961,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>J28</t>
+          <t>J17</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -971,7 +971,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>613.6000000000008</v>
+        <v>2628.199999999998</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -985,7 +985,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>J29</t>
+          <t>J23</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -995,7 +995,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>626.5000000000014</v>
+        <v>2734.299999999998</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1009,11 +1009,467 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>J25</t>
+          <t>J20</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>2840.399999999998</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>J6</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>3051.599999999998</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>J14</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3177.799999999998</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>J15</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>3183.799999999998</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>J2</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>3233.099999999998</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>J6</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>3384.299999999997</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>J27</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3465.399999999997</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>J26</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>3570.699999999997</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>J20</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3601.699999999997</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>J17</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>3625.899999999997</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>J16</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>3730.999999999997</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>J19</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>3793.099999999997</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>J8</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>3899.199999999997</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>J4</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>4258.899999999996</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>J30</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>4264.899999999996</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>J4</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>4444.199999999997</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>J15</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>4592.799999999999</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>J23</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>4740.200000000001</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>J26</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>4925.700000000003</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>fetch_request</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>J26</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>